<commit_message>
import DateTime for matches
</commit_message>
<xml_diff>
--- a/testresources/match.xlsx
+++ b/testresources/match.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Typer\testresources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13A725B8-01F1-42DA-BFCF-4D21000A84E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F64CB71-8944-4474-BE0E-5C3AB3510142}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32760" yWindow="32760" windowWidth="20736" windowHeight="8726"/>
+    <workbookView xWindow="32760" yWindow="32760" windowWidth="20736" windowHeight="8726" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>roundId</t>
   </si>
@@ -37,12 +37,18 @@
   <si>
     <t>awayTeamId</t>
   </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>2018-10-18T21:15:30.00Z</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,6 +65,13 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF6A8759"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -82,9 +95,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
@@ -399,20 +415,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -422,8 +440,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -432,12 +453,16 @@
       </c>
       <c r="C2">
         <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="poczta@o2.pl"/>
+    <hyperlink ref="A2" r:id="rId1" display="poczta@o2.pl" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>